<commit_message>
added water wash hods
</commit_message>
<xml_diff>
--- a/T&C.xlsx
+++ b/T&C.xlsx
@@ -546,7 +546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
@@ -596,14 +596,14 @@
     <row r="10">
       <c r="A10" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">DATE OF VISIT: 2024-09-28 </t>
+          <t xml:space="preserve">DATE OF VISIT: 2024-10-01 </t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">ENGINEER(s):  </t>
+          <t xml:space="preserve">ENGINEER(s): Mike, Yazan </t>
         </is>
       </c>
     </row>
@@ -632,7 +632,7 @@
     <row r="17">
       <c r="A17" s="8" t="inlineStr">
         <is>
-          <t>Drawing Number: 	212</t>
+          <t>Drawing Number: 	1212</t>
         </is>
       </c>
       <c r="B17" s="9" t="n"/>
@@ -647,7 +647,7 @@
     <row r="18">
       <c r="A18" s="8" t="inlineStr">
         <is>
-          <t>Location: 	dee</t>
+          <t>Location: 	Main Kitchen</t>
         </is>
       </c>
       <c r="B18" s="9" t="n"/>
@@ -662,7 +662,7 @@
     <row r="19">
       <c r="A19" s="8" t="inlineStr">
         <is>
-          <t>Model: 	KSR-F</t>
+          <t>Model: 	KCH-I</t>
         </is>
       </c>
       <c r="B19" s="9" t="n"/>
@@ -677,7 +677,7 @@
     <row r="20">
       <c r="A20" s="8" t="inlineStr">
         <is>
-          <t>Quantity of Canopy Sections: 	1</t>
+          <t>Quantity of Canopy Sections: 	2</t>
         </is>
       </c>
       <c r="B20" s="9" t="n"/>
@@ -762,93 +762,113 @@
       </c>
       <c r="B24" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 33.0 pa</t>
+          <t xml:space="preserve"> 300.0 pa</t>
         </is>
       </c>
       <c r="C24" s="12" t="n"/>
       <c r="D24" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 67.7</t>
+          <t xml:space="preserve"> 215.4</t>
         </is>
       </c>
       <c r="E24" s="12" t="n"/>
       <c r="F24" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 388.91</t>
+          <t xml:space="preserve"> 3730.84</t>
         </is>
       </c>
       <c r="G24" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 212.0</t>
+          <t xml:space="preserve"> 400.0</t>
         </is>
       </c>
       <c r="H24" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 2.0%</t>
+          <t xml:space="preserve"> 9.0%</t>
         </is>
       </c>
       <c r="I24" s="12" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="13" t="n"/>
-      <c r="B25" s="13" t="n"/>
-      <c r="C25" s="13" t="n"/>
-      <c r="D25" s="13" t="n"/>
+      <c r="A25" s="11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B25" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 322.0 pa</t>
+        </is>
+      </c>
+      <c r="C25" s="12" t="n"/>
+      <c r="D25" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 143.6</t>
+        </is>
+      </c>
+      <c r="E25" s="12" t="n"/>
+      <c r="F25" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2576.81</t>
+        </is>
+      </c>
+      <c r="G25" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 323.0</t>
+        </is>
+      </c>
+      <c r="H25" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 8.0%</t>
+        </is>
+      </c>
+      <c r="I25" s="12" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="14" t="inlineStr">
-        <is>
-          <t>Total Flowrate                                212.0 m3/s</t>
-        </is>
-      </c>
-      <c r="B26" s="12" t="n"/>
-      <c r="C26" s="12" t="n"/>
-      <c r="D26" s="12" t="n"/>
+      <c r="A26" s="13" t="n"/>
+      <c r="B26" s="13" t="n"/>
+      <c r="C26" s="13" t="n"/>
+      <c r="D26" s="13" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="14" t="inlineStr">
         <is>
-          <t>Total Percentage                                55.0%</t>
+          <t>Total Flowrate                                723.0 m3/s</t>
         </is>
       </c>
       <c r="B27" s="12" t="n"/>
       <c r="C27" s="12" t="n"/>
       <c r="D27" s="12" t="n"/>
     </row>
-    <row r="29">
-      <c r="A29" s="6" t="inlineStr">
-        <is>
-          <t>SUPPLY AIR DATA</t>
-        </is>
-      </c>
-      <c r="B29" s="7" t="n"/>
-      <c r="C29" s="7" t="n"/>
-      <c r="D29" s="7" t="n"/>
-      <c r="E29" s="7" t="n"/>
-      <c r="F29" s="7" t="n"/>
-      <c r="G29" s="7" t="n"/>
-      <c r="H29" s="7" t="n"/>
-      <c r="I29" s="7" t="n"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="8" t="inlineStr">
-        <is>
-          <t>Drawing Number: 	212</t>
-        </is>
-      </c>
-      <c r="B30" s="9" t="n"/>
-      <c r="C30" s="9" t="n"/>
-      <c r="D30" s="9" t="n"/>
-      <c r="E30" s="9" t="n"/>
-      <c r="F30" s="9" t="n"/>
-      <c r="G30" s="9" t="n"/>
-      <c r="H30" s="9" t="n"/>
-      <c r="I30" s="10" t="n"/>
+    <row r="28">
+      <c r="A28" s="14" t="inlineStr">
+        <is>
+          <t>Total Percentage                                11.0%</t>
+        </is>
+      </c>
+      <c r="B28" s="12" t="n"/>
+      <c r="C28" s="12" t="n"/>
+      <c r="D28" s="12" t="n"/>
+    </row>
+    <row r="30" ht="20" customHeight="1">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>EXTRACT AIR DATA</t>
+        </is>
+      </c>
+      <c r="B30" s="7" t="n"/>
+      <c r="C30" s="7" t="n"/>
+      <c r="D30" s="7" t="n"/>
+      <c r="E30" s="7" t="n"/>
+      <c r="F30" s="7" t="n"/>
+      <c r="G30" s="7" t="n"/>
+      <c r="H30" s="7" t="n"/>
+      <c r="I30" s="7" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="8" t="inlineStr">
         <is>
-          <t>Location: 	dee</t>
+          <t xml:space="preserve">Drawing Number: 	</t>
         </is>
       </c>
       <c r="B31" s="9" t="n"/>
@@ -863,7 +883,7 @@
     <row r="32">
       <c r="A32" s="8" t="inlineStr">
         <is>
-          <t>Model: 	KSR-F</t>
+          <t xml:space="preserve">Location: 	</t>
         </is>
       </c>
       <c r="B32" s="9" t="n"/>
@@ -878,7 +898,7 @@
     <row r="33">
       <c r="A33" s="8" t="inlineStr">
         <is>
-          <t>Quantity of Canopy Sections: 	1</t>
+          <t>Model: 	KVI</t>
         </is>
       </c>
       <c r="B33" s="9" t="n"/>
@@ -893,7 +913,7 @@
     <row r="34">
       <c r="A34" s="8" t="inlineStr">
         <is>
-          <t>Calculation: 	QV = Kf x √Pa</t>
+          <t>Quantity of Canopy Sections: 	1</t>
         </is>
       </c>
       <c r="B34" s="9" t="n"/>
@@ -906,144 +926,375 @@
       <c r="I34" s="10" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="6" t="inlineStr">
-        <is>
-          <t>SUPPLY AIR READINGS</t>
-        </is>
-      </c>
-      <c r="B35" s="7" t="n"/>
-      <c r="C35" s="7" t="n"/>
-      <c r="D35" s="7" t="n"/>
-      <c r="E35" s="7" t="n"/>
-      <c r="F35" s="7" t="n"/>
-      <c r="G35" s="7" t="n"/>
-      <c r="H35" s="7" t="n"/>
-      <c r="I35" s="7" t="n"/>
-    </row>
-    <row r="36" ht="30" customHeight="1">
-      <c r="A36" s="11" t="inlineStr">
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t>Calculation: 	QV = Kf x √Pa</t>
+        </is>
+      </c>
+      <c r="B35" s="9" t="n"/>
+      <c r="C35" s="9" t="n"/>
+      <c r="D35" s="9" t="n"/>
+      <c r="E35" s="9" t="n"/>
+      <c r="F35" s="9" t="n"/>
+      <c r="G35" s="9" t="n"/>
+      <c r="H35" s="9" t="n"/>
+      <c r="I35" s="10" t="n"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="inlineStr">
+        <is>
+          <t>EXTRACT AIR READINGS</t>
+        </is>
+      </c>
+      <c r="B36" s="7" t="n"/>
+      <c r="C36" s="7" t="n"/>
+      <c r="D36" s="7" t="n"/>
+      <c r="E36" s="7" t="n"/>
+      <c r="F36" s="7" t="n"/>
+      <c r="G36" s="7" t="n"/>
+      <c r="H36" s="7" t="n"/>
+      <c r="I36" s="7" t="n"/>
+    </row>
+    <row r="37" ht="30" customHeight="1">
+      <c r="A37" s="11" t="inlineStr">
         <is>
           <t>Module #</t>
         </is>
       </c>
-      <c r="B36" s="11" t="inlineStr">
+      <c r="B37" s="11" t="inlineStr">
         <is>
           <t>T.A.B Point Reading (Pa)</t>
-        </is>
-      </c>
-      <c r="C36" s="12" t="n"/>
-      <c r="D36" s="11" t="inlineStr">
-        <is>
-          <t>K-Factor (m3 /h)</t>
-        </is>
-      </c>
-      <c r="E36" s="12" t="n"/>
-      <c r="F36" s="11" t="inlineStr">
-        <is>
-          <t>Flowrate (m3 /h)</t>
-        </is>
-      </c>
-      <c r="G36" s="11" t="inlineStr">
-        <is>
-          <t>Flowrate (m3 /s)</t>
-        </is>
-      </c>
-      <c r="H36" s="11" t="inlineStr">
-        <is>
-          <t>Percentage</t>
-        </is>
-      </c>
-      <c r="I36" s="12" t="n"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B37" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 23.0 pa</t>
         </is>
       </c>
       <c r="C37" s="12" t="n"/>
       <c r="D37" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 121.7</t>
+          <t>K-Factor (m3 /h)</t>
         </is>
       </c>
       <c r="E37" s="12" t="n"/>
       <c r="F37" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 583.65</t>
+          <t>Flowrate (m3 /h)</t>
         </is>
       </c>
       <c r="G37" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 23.0</t>
+          <t>Flowrate (m3 /s)</t>
         </is>
       </c>
       <c r="H37" s="11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 25.0%</t>
+          <t>Percentage</t>
         </is>
       </c>
       <c r="I37" s="12" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="13" t="n"/>
-      <c r="B38" s="13" t="n"/>
-      <c r="C38" s="13" t="n"/>
-      <c r="D38" s="13" t="n"/>
+      <c r="A38" s="11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B38" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 23.0 pa</t>
+        </is>
+      </c>
+      <c r="C38" s="12" t="n"/>
+      <c r="D38" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 71.8</t>
+        </is>
+      </c>
+      <c r="E38" s="12" t="n"/>
+      <c r="F38" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 344.34</t>
+        </is>
+      </c>
+      <c r="G38" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 32.0</t>
+        </is>
+      </c>
+      <c r="H38" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11.0%</t>
+        </is>
+      </c>
+      <c r="I38" s="12" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="14" t="inlineStr">
-        <is>
-          <t>Total Flowrate                                23.0 m3/s</t>
-        </is>
-      </c>
-      <c r="B39" s="12" t="n"/>
-      <c r="C39" s="12" t="n"/>
-      <c r="D39" s="12" t="n"/>
+      <c r="A39" s="13" t="n"/>
+      <c r="B39" s="13" t="n"/>
+      <c r="C39" s="13" t="n"/>
+      <c r="D39" s="13" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="14" t="inlineStr">
         <is>
-          <t>Total Percentage                                25.0%</t>
+          <t>Total Flowrate                                32.0 m3/s</t>
         </is>
       </c>
       <c r="B40" s="12" t="n"/>
       <c r="C40" s="12" t="n"/>
       <c r="D40" s="12" t="n"/>
     </row>
+    <row r="41">
+      <c r="A41" s="14" t="inlineStr">
+        <is>
+          <t>Total Percentage                                9.0%</t>
+        </is>
+      </c>
+      <c r="B41" s="12" t="n"/>
+      <c r="C41" s="12" t="n"/>
+      <c r="D41" s="12" t="n"/>
+    </row>
+    <row r="43" ht="20" customHeight="1">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>EXTRACT AIR DATA</t>
+        </is>
+      </c>
+      <c r="B43" s="7" t="n"/>
+      <c r="C43" s="7" t="n"/>
+      <c r="D43" s="7" t="n"/>
+      <c r="E43" s="7" t="n"/>
+      <c r="F43" s="7" t="n"/>
+      <c r="G43" s="7" t="n"/>
+      <c r="H43" s="7" t="n"/>
+      <c r="I43" s="7" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Drawing Number: 	</t>
+        </is>
+      </c>
+      <c r="B44" s="9" t="n"/>
+      <c r="C44" s="9" t="n"/>
+      <c r="D44" s="9" t="n"/>
+      <c r="E44" s="9" t="n"/>
+      <c r="F44" s="9" t="n"/>
+      <c r="G44" s="9" t="n"/>
+      <c r="H44" s="9" t="n"/>
+      <c r="I44" s="10" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Location: 	</t>
+        </is>
+      </c>
+      <c r="B45" s="9" t="n"/>
+      <c r="C45" s="9" t="n"/>
+      <c r="D45" s="9" t="n"/>
+      <c r="E45" s="9" t="n"/>
+      <c r="F45" s="9" t="n"/>
+      <c r="G45" s="9" t="n"/>
+      <c r="H45" s="9" t="n"/>
+      <c r="I45" s="10" t="n"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="8" t="inlineStr">
+        <is>
+          <t>Model: 	KVI</t>
+        </is>
+      </c>
+      <c r="B46" s="9" t="n"/>
+      <c r="C46" s="9" t="n"/>
+      <c r="D46" s="9" t="n"/>
+      <c r="E46" s="9" t="n"/>
+      <c r="F46" s="9" t="n"/>
+      <c r="G46" s="9" t="n"/>
+      <c r="H46" s="9" t="n"/>
+      <c r="I46" s="10" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="8" t="inlineStr">
+        <is>
+          <t>Quantity of Canopy Sections: 	1</t>
+        </is>
+      </c>
+      <c r="B47" s="9" t="n"/>
+      <c r="C47" s="9" t="n"/>
+      <c r="D47" s="9" t="n"/>
+      <c r="E47" s="9" t="n"/>
+      <c r="F47" s="9" t="n"/>
+      <c r="G47" s="9" t="n"/>
+      <c r="H47" s="9" t="n"/>
+      <c r="I47" s="10" t="n"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="8" t="inlineStr">
+        <is>
+          <t>Calculation: 	QV = Kf x √Pa</t>
+        </is>
+      </c>
+      <c r="B48" s="9" t="n"/>
+      <c r="C48" s="9" t="n"/>
+      <c r="D48" s="9" t="n"/>
+      <c r="E48" s="9" t="n"/>
+      <c r="F48" s="9" t="n"/>
+      <c r="G48" s="9" t="n"/>
+      <c r="H48" s="9" t="n"/>
+      <c r="I48" s="10" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>EXTRACT AIR READINGS</t>
+        </is>
+      </c>
+      <c r="B49" s="7" t="n"/>
+      <c r="C49" s="7" t="n"/>
+      <c r="D49" s="7" t="n"/>
+      <c r="E49" s="7" t="n"/>
+      <c r="F49" s="7" t="n"/>
+      <c r="G49" s="7" t="n"/>
+      <c r="H49" s="7" t="n"/>
+      <c r="I49" s="7" t="n"/>
+    </row>
+    <row r="50" ht="30" customHeight="1">
+      <c r="A50" s="11" t="inlineStr">
+        <is>
+          <t>Module #</t>
+        </is>
+      </c>
+      <c r="B50" s="11" t="inlineStr">
+        <is>
+          <t>T.A.B Point Reading (Pa)</t>
+        </is>
+      </c>
+      <c r="C50" s="12" t="n"/>
+      <c r="D50" s="11" t="inlineStr">
+        <is>
+          <t>K-Factor (m3 /h)</t>
+        </is>
+      </c>
+      <c r="E50" s="12" t="n"/>
+      <c r="F50" s="11" t="inlineStr">
+        <is>
+          <t>Flowrate (m3 /h)</t>
+        </is>
+      </c>
+      <c r="G50" s="11" t="inlineStr">
+        <is>
+          <t>Flowrate (m3 /s)</t>
+        </is>
+      </c>
+      <c r="H50" s="11" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="I50" s="12" t="n"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B51" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 322.0 pa</t>
+        </is>
+      </c>
+      <c r="C51" s="12" t="n"/>
+      <c r="D51" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 71.8</t>
+        </is>
+      </c>
+      <c r="E51" s="12" t="n"/>
+      <c r="F51" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1288.4</t>
+        </is>
+      </c>
+      <c r="G51" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 33.0</t>
+        </is>
+      </c>
+      <c r="H51" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 39.0%</t>
+        </is>
+      </c>
+      <c r="I51" s="12" t="n"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="13" t="n"/>
+      <c r="B52" s="13" t="n"/>
+      <c r="C52" s="13" t="n"/>
+      <c r="D52" s="13" t="n"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="14" t="inlineStr">
+        <is>
+          <t>Total Flowrate                                33.0 m3/s</t>
+        </is>
+      </c>
+      <c r="B53" s="12" t="n"/>
+      <c r="C53" s="12" t="n"/>
+      <c r="D53" s="12" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="14" t="inlineStr">
+        <is>
+          <t>Total Percentage                                3.0%</t>
+        </is>
+      </c>
+      <c r="B54" s="12" t="n"/>
+      <c r="C54" s="12" t="n"/>
+      <c r="D54" s="12" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="D36:E36"/>
+  <mergeCells count="33">
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="H25:I25"/>
     <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A39:D39"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H51:I51"/>
     <mergeCell ref="A22:I22"/>
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="A43:I43"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A54:D54"/>
     <mergeCell ref="H37:I37"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A30:I30"/>
+    <mergeCell ref="D25:E25"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A49:I49"/>
     <mergeCell ref="H24:I24"/>
-    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
     <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
     <mergeCell ref="A16:I16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <rowBreaks count="2" manualBreakCount="2">
+  <rowBreaks count="4" manualBreakCount="4">
     <brk id="12" min="0" max="16383" man="1"/>
-    <brk id="42" min="0" max="16383" man="1"/>
+    <brk id="28" min="0" max="16383" man="1"/>
+    <brk id="41" min="0" max="16383" man="1"/>
+    <brk id="54" min="0" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>